<commit_message>
before modifying process function
</commit_message>
<xml_diff>
--- a/outputs/u/_colander_both.xlsx
+++ b/outputs/u/_colander_both.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="269">
   <si>
     <t>participant</t>
   </si>
@@ -45,9 +45,6 @@
     <t>place</t>
   </si>
   <si>
-    <t>activity</t>
-  </si>
-  <si>
     <t>reg</t>
   </si>
   <si>
@@ -814,6 +811,21 @@
   </si>
   <si>
     <t>items_uniq</t>
+  </si>
+  <si>
+    <t>place_1</t>
+  </si>
+  <si>
+    <t>place_2</t>
+  </si>
+  <si>
+    <t>activity_1</t>
+  </si>
+  <si>
+    <t>type_1</t>
+  </si>
+  <si>
+    <t>type_2</t>
   </si>
 </sst>
 </file>
@@ -1632,18 +1644,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W126"/>
+  <dimension ref="A1:Y126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:W1048576"/>
+      <selection activeCell="I1" sqref="I1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="11" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="6" max="8" width="9.140625" customWidth="1"/>
+    <col min="11" max="14" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1666,46 +1680,55 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>264</v>
+      </c>
+      <c r="J1" t="s">
+        <v>265</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="N1" t="s">
+        <v>266</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="P1" t="s">
         <v>0</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>1</v>
       </c>
-      <c r="P1" t="s">
-        <v>264</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
+        <v>263</v>
+      </c>
+      <c r="S1" t="s">
         <v>2</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>3</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>4</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>5</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>6</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
+        <v>256</v>
+      </c>
+      <c r="Y1" t="s">
         <v>257</v>
       </c>
-      <c r="W1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1713,7 +1736,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>220</v>
@@ -1725,49 +1748,55 @@
         <v>1788</v>
       </c>
       <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="N2">
+      <c r="K2" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="M2" t="s">
+        <v>258</v>
+      </c>
+      <c r="N2" t="s">
+        <v>259</v>
+      </c>
+      <c r="P2">
         <v>4</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>220</v>
+      </c>
+      <c r="T2">
+        <v>1782</v>
+      </c>
+      <c r="U2">
+        <v>1788</v>
+      </c>
+      <c r="V2" t="s">
         <v>9</v>
       </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>220</v>
-      </c>
-      <c r="R2">
-        <v>1782</v>
-      </c>
-      <c r="S2">
-        <v>1788</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="W2" t="s">
         <v>10</v>
       </c>
-      <c r="U2" t="s">
-        <v>11</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
+        <v>258</v>
+      </c>
+      <c r="Y2" t="s">
         <v>259</v>
       </c>
-      <c r="W2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1775,7 +1804,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>33</v>
@@ -1787,49 +1816,55 @@
         <v>412</v>
       </c>
       <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="N3">
-        <v>8</v>
-      </c>
-      <c r="O3" t="s">
-        <v>9</v>
+      <c r="K3" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="M3" t="s">
+        <v>258</v>
+      </c>
+      <c r="N3" t="s">
+        <v>259</v>
       </c>
       <c r="P3">
+        <v>8</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3">
         <v>0</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>33</v>
       </c>
-      <c r="R3">
+      <c r="T3">
         <v>374</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <v>412</v>
       </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
+        <v>12</v>
+      </c>
+      <c r="W3" t="s">
         <v>13</v>
       </c>
-      <c r="U3" t="s">
-        <v>14</v>
-      </c>
-      <c r="V3" t="s">
+      <c r="X3" t="s">
+        <v>258</v>
+      </c>
+      <c r="Y3" t="s">
         <v>259</v>
       </c>
-      <c r="W3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1837,7 +1872,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>247</v>
@@ -1849,49 +1884,55 @@
         <v>2582</v>
       </c>
       <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
         <v>16</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>17</v>
       </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="N4">
+      <c r="K4" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="M4" t="s">
+        <v>258</v>
+      </c>
+      <c r="N4" t="s">
+        <v>260</v>
+      </c>
+      <c r="P4">
         <v>11</v>
       </c>
-      <c r="O4" t="s">
-        <v>9</v>
-      </c>
-      <c r="P4">
+      <c r="Q4" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4">
         <v>0</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>247</v>
       </c>
-      <c r="R4">
+      <c r="T4">
         <v>2558</v>
       </c>
-      <c r="S4">
+      <c r="U4">
         <v>2582</v>
       </c>
-      <c r="T4" t="s">
+      <c r="V4" t="s">
+        <v>15</v>
+      </c>
+      <c r="W4" t="s">
         <v>16</v>
       </c>
-      <c r="U4" t="s">
-        <v>17</v>
-      </c>
-      <c r="V4" t="s">
-        <v>259</v>
-      </c>
-      <c r="W4" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X4" t="s">
+        <v>258</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1899,7 +1940,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <v>45</v>
@@ -1911,52 +1952,58 @@
         <v>410</v>
       </c>
       <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
         <v>19</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>20</v>
       </c>
-      <c r="I5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="N5">
+      <c r="M5" t="s">
+        <v>261</v>
+      </c>
+      <c r="N5" t="s">
+        <v>259</v>
+      </c>
+      <c r="P5">
         <v>12</v>
       </c>
-      <c r="O5" t="s">
-        <v>9</v>
-      </c>
-      <c r="P5">
+      <c r="Q5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R5">
         <v>0</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>32</v>
       </c>
-      <c r="R5">
+      <c r="T5">
         <v>338</v>
       </c>
-      <c r="S5">
+      <c r="U5">
         <v>340</v>
       </c>
-      <c r="T5" t="s">
+      <c r="V5" t="s">
+        <v>63</v>
+      </c>
+      <c r="W5" t="s">
         <v>64</v>
       </c>
-      <c r="U5" t="s">
-        <v>65</v>
-      </c>
-      <c r="V5" t="s">
-        <v>262</v>
-      </c>
-      <c r="W5" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X5" t="s">
+        <v>261</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1964,7 +2011,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>349</v>
@@ -1976,49 +2023,55 @@
         <v>3784</v>
       </c>
       <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" t="s">
         <v>22</v>
       </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
       <c r="I6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="N6">
+        <v>20</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="M6" t="s">
+        <v>261</v>
+      </c>
+      <c r="N6" t="s">
+        <v>259</v>
+      </c>
+      <c r="P6">
         <v>17</v>
       </c>
-      <c r="O6" t="s">
-        <v>9</v>
-      </c>
-      <c r="P6">
+      <c r="Q6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R6">
         <v>0</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>87</v>
       </c>
-      <c r="R6">
+      <c r="T6">
         <v>1206</v>
       </c>
-      <c r="S6">
+      <c r="U6">
         <v>1228</v>
       </c>
-      <c r="T6" t="s">
+      <c r="V6" t="s">
+        <v>88</v>
+      </c>
+      <c r="W6" t="s">
         <v>89</v>
       </c>
-      <c r="U6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V6" t="s">
+      <c r="X6" t="s">
+        <v>258</v>
+      </c>
+      <c r="Y6" t="s">
         <v>259</v>
       </c>
-      <c r="W6" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2026,7 +2079,7 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>124</v>
@@ -2038,49 +2091,55 @@
         <v>1494</v>
       </c>
       <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s">
         <v>24</v>
       </c>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
       <c r="I7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M7" t="s">
+        <v>258</v>
+      </c>
+      <c r="N7" t="s">
+        <v>259</v>
+      </c>
+      <c r="P7">
         <v>18</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="N7">
-        <v>18</v>
-      </c>
-      <c r="O7" t="s">
-        <v>9</v>
-      </c>
-      <c r="P7">
+      <c r="Q7" t="s">
+        <v>8</v>
+      </c>
+      <c r="R7">
         <v>0</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <v>490</v>
       </c>
-      <c r="R7">
+      <c r="T7">
         <v>2246</v>
       </c>
-      <c r="S7">
+      <c r="U7">
         <v>2252</v>
       </c>
-      <c r="T7" t="s">
+      <c r="V7" t="s">
+        <v>110</v>
+      </c>
+      <c r="W7" t="s">
         <v>111</v>
       </c>
-      <c r="U7" t="s">
-        <v>112</v>
-      </c>
-      <c r="V7" t="s">
+      <c r="X7" t="s">
+        <v>258</v>
+      </c>
+      <c r="Y7" t="s">
         <v>259</v>
       </c>
-      <c r="W7" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2088,7 +2147,7 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>491</v>
@@ -2100,49 +2159,55 @@
         <v>4336</v>
       </c>
       <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" t="s">
         <v>26</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>27</v>
       </c>
-      <c r="I8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N8">
+      <c r="M8" t="s">
+        <v>258</v>
+      </c>
+      <c r="N8" t="s">
+        <v>259</v>
+      </c>
+      <c r="P8">
         <v>19</v>
       </c>
-      <c r="O8" t="s">
-        <v>9</v>
-      </c>
-      <c r="P8">
+      <c r="Q8" t="s">
+        <v>8</v>
+      </c>
+      <c r="R8">
         <v>0</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <v>199</v>
       </c>
-      <c r="R8">
+      <c r="T8">
         <v>1548</v>
       </c>
-      <c r="S8">
+      <c r="U8">
         <v>1550</v>
       </c>
-      <c r="T8" t="s">
+      <c r="V8" t="s">
+        <v>116</v>
+      </c>
+      <c r="W8" t="s">
         <v>117</v>
       </c>
-      <c r="U8" t="s">
-        <v>118</v>
-      </c>
-      <c r="V8" t="s">
+      <c r="X8" t="s">
+        <v>258</v>
+      </c>
+      <c r="Y8" t="s">
         <v>259</v>
       </c>
-      <c r="W8" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2150,7 +2215,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>513</v>
@@ -2162,49 +2227,55 @@
         <v>2324</v>
       </c>
       <c r="G9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" t="s">
         <v>29</v>
       </c>
-      <c r="H9" t="s">
-        <v>30</v>
-      </c>
       <c r="I9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="N9">
+        <v>27</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="M9" t="s">
+        <v>258</v>
+      </c>
+      <c r="N9" t="s">
+        <v>259</v>
+      </c>
+      <c r="P9">
         <v>20</v>
       </c>
-      <c r="O9" t="s">
-        <v>9</v>
-      </c>
-      <c r="P9">
+      <c r="Q9" t="s">
+        <v>8</v>
+      </c>
+      <c r="R9">
         <v>0</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <v>145</v>
       </c>
-      <c r="R9">
+      <c r="T9">
         <v>972</v>
       </c>
-      <c r="S9">
+      <c r="U9">
         <v>978</v>
       </c>
-      <c r="T9" t="s">
+      <c r="V9" t="s">
+        <v>125</v>
+      </c>
+      <c r="W9" t="s">
         <v>126</v>
       </c>
-      <c r="U9" t="s">
-        <v>127</v>
-      </c>
-      <c r="V9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W9" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X9" t="s">
+        <v>258</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2212,7 +2283,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <v>346</v>
@@ -2224,49 +2295,55 @@
         <v>2398</v>
       </c>
       <c r="G10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" t="s">
         <v>31</v>
       </c>
-      <c r="H10" t="s">
-        <v>32</v>
-      </c>
       <c r="I10" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="N10">
+        <v>14</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="M10" t="s">
+        <v>258</v>
+      </c>
+      <c r="N10" t="s">
+        <v>259</v>
+      </c>
+      <c r="P10">
         <v>2</v>
       </c>
-      <c r="O10" t="s">
-        <v>39</v>
-      </c>
-      <c r="P10">
+      <c r="Q10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R10">
         <v>0</v>
       </c>
-      <c r="Q10">
+      <c r="S10">
         <v>133</v>
       </c>
-      <c r="R10">
+      <c r="T10">
         <v>2170</v>
       </c>
-      <c r="S10">
+      <c r="U10">
         <v>2174</v>
       </c>
-      <c r="T10" t="s">
+      <c r="V10" t="s">
+        <v>162</v>
+      </c>
+      <c r="W10" t="s">
         <v>163</v>
       </c>
-      <c r="U10" t="s">
-        <v>164</v>
-      </c>
-      <c r="V10" t="s">
+      <c r="X10" t="s">
+        <v>258</v>
+      </c>
+      <c r="Y10" t="s">
         <v>259</v>
       </c>
-      <c r="W10" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2274,7 +2351,7 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11">
         <v>158</v>
@@ -2286,49 +2363,55 @@
         <v>1058</v>
       </c>
       <c r="G11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" t="s">
         <v>33</v>
       </c>
-      <c r="H11" t="s">
-        <v>34</v>
-      </c>
       <c r="I11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="N11">
+        <v>17</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="M11" t="s">
+        <v>258</v>
+      </c>
+      <c r="N11" t="s">
+        <v>260</v>
+      </c>
+      <c r="P11">
         <v>5</v>
       </c>
-      <c r="O11" t="s">
-        <v>39</v>
-      </c>
-      <c r="P11">
+      <c r="Q11" t="s">
+        <v>38</v>
+      </c>
+      <c r="R11">
         <v>0</v>
       </c>
-      <c r="Q11">
+      <c r="S11">
         <v>5</v>
       </c>
-      <c r="R11">
+      <c r="T11">
         <v>32</v>
       </c>
-      <c r="S11">
+      <c r="U11">
         <v>52</v>
       </c>
-      <c r="T11" t="s">
+      <c r="V11" t="s">
+        <v>41</v>
+      </c>
+      <c r="W11" t="s">
         <v>42</v>
       </c>
-      <c r="U11" t="s">
-        <v>43</v>
-      </c>
-      <c r="V11" t="s">
+      <c r="X11" t="s">
+        <v>258</v>
+      </c>
+      <c r="Y11" t="s">
         <v>259</v>
       </c>
-      <c r="W11" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2336,7 +2419,7 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12">
         <v>190</v>
@@ -2348,49 +2431,55 @@
         <v>1540</v>
       </c>
       <c r="G12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" t="s">
         <v>35</v>
       </c>
-      <c r="H12" t="s">
-        <v>36</v>
-      </c>
       <c r="I12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="N12">
+        <v>14</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M12" t="s">
+        <v>258</v>
+      </c>
+      <c r="N12" t="s">
+        <v>260</v>
+      </c>
+      <c r="P12">
         <v>12</v>
       </c>
-      <c r="O12" t="s">
-        <v>39</v>
-      </c>
-      <c r="P12">
+      <c r="Q12" t="s">
+        <v>38</v>
+      </c>
+      <c r="R12">
         <v>0</v>
       </c>
-      <c r="Q12">
+      <c r="S12">
         <v>49</v>
       </c>
-      <c r="R12">
+      <c r="T12">
         <v>500</v>
       </c>
-      <c r="S12">
+      <c r="U12">
         <v>506</v>
       </c>
-      <c r="T12" t="s">
+      <c r="V12" t="s">
+        <v>173</v>
+      </c>
+      <c r="W12" t="s">
         <v>174</v>
       </c>
-      <c r="U12" t="s">
-        <v>175</v>
-      </c>
-      <c r="V12" t="s">
+      <c r="X12" t="s">
+        <v>261</v>
+      </c>
+      <c r="Y12" t="s">
         <v>262</v>
       </c>
-      <c r="W12" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2398,7 +2487,7 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13">
         <v>509</v>
@@ -2410,52 +2499,58 @@
         <v>3422</v>
       </c>
       <c r="G13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" t="s">
         <v>37</v>
       </c>
-      <c r="H13" t="s">
-        <v>38</v>
-      </c>
       <c r="I13" t="s">
-        <v>28</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>248</v>
+        <v>27</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="N13">
+        <v>247</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="M13" t="s">
+        <v>258</v>
+      </c>
+      <c r="N13" t="s">
+        <v>260</v>
+      </c>
+      <c r="P13">
         <v>15</v>
       </c>
-      <c r="O13" t="s">
-        <v>39</v>
-      </c>
-      <c r="P13">
+      <c r="Q13" t="s">
+        <v>38</v>
+      </c>
+      <c r="R13">
         <v>0</v>
       </c>
-      <c r="Q13">
+      <c r="S13">
         <v>398</v>
       </c>
-      <c r="R13">
+      <c r="T13">
         <v>2480</v>
       </c>
-      <c r="S13">
+      <c r="U13">
         <v>2494</v>
       </c>
-      <c r="T13" t="s">
+      <c r="V13" t="s">
+        <v>45</v>
+      </c>
+      <c r="W13" t="s">
         <v>46</v>
       </c>
-      <c r="U13" t="s">
-        <v>47</v>
-      </c>
-      <c r="V13" t="s">
+      <c r="X13" t="s">
+        <v>258</v>
+      </c>
+      <c r="Y13" t="s">
         <v>259</v>
       </c>
-      <c r="W13" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2463,7 +2558,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14">
         <v>411</v>
@@ -2475,52 +2570,58 @@
         <v>4810</v>
       </c>
       <c r="G14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" t="s">
         <v>40</v>
       </c>
-      <c r="H14" t="s">
-        <v>41</v>
-      </c>
       <c r="I14" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="N14">
+        <v>14</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="M14" t="s">
+        <v>258</v>
+      </c>
+      <c r="N14" t="s">
+        <v>259</v>
+      </c>
+      <c r="P14">
         <v>17</v>
       </c>
-      <c r="O14" t="s">
-        <v>39</v>
-      </c>
-      <c r="P14">
+      <c r="Q14" t="s">
+        <v>38</v>
+      </c>
+      <c r="R14">
         <v>0</v>
       </c>
-      <c r="Q14">
+      <c r="S14">
         <v>55</v>
       </c>
-      <c r="R14">
+      <c r="T14">
         <v>1036</v>
       </c>
-      <c r="S14">
+      <c r="U14">
         <v>1044</v>
       </c>
-      <c r="T14" t="s">
-        <v>186</v>
-      </c>
-      <c r="U14" t="s">
-        <v>131</v>
-      </c>
       <c r="V14" t="s">
+        <v>185</v>
+      </c>
+      <c r="W14" t="s">
+        <v>130</v>
+      </c>
+      <c r="X14" t="s">
+        <v>258</v>
+      </c>
+      <c r="Y14" t="s">
         <v>259</v>
       </c>
-      <c r="W14" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2528,7 +2629,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -2540,49 +2641,55 @@
         <v>52</v>
       </c>
       <c r="G15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" t="s">
         <v>42</v>
       </c>
-      <c r="H15" t="s">
-        <v>43</v>
-      </c>
       <c r="I15" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="M15" t="s">
+        <v>258</v>
+      </c>
+      <c r="N15" t="s">
+        <v>259</v>
+      </c>
+      <c r="P15">
         <v>18</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="N15">
-        <v>18</v>
-      </c>
-      <c r="O15" t="s">
-        <v>39</v>
-      </c>
-      <c r="P15">
+      <c r="Q15" t="s">
+        <v>38</v>
+      </c>
+      <c r="R15">
         <v>0</v>
       </c>
-      <c r="Q15">
+      <c r="S15">
         <v>228</v>
       </c>
-      <c r="R15">
+      <c r="T15">
         <v>1350</v>
       </c>
-      <c r="S15">
+      <c r="U15">
         <v>1356</v>
       </c>
-      <c r="T15" t="s">
-        <v>198</v>
-      </c>
-      <c r="U15" t="s">
-        <v>209</v>
-      </c>
       <c r="V15" t="s">
+        <v>197</v>
+      </c>
+      <c r="W15" t="s">
+        <v>208</v>
+      </c>
+      <c r="X15" t="s">
+        <v>258</v>
+      </c>
+      <c r="Y15" t="s">
         <v>259</v>
       </c>
-      <c r="W15" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2590,7 +2697,7 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16">
         <v>241</v>
@@ -2602,49 +2709,55 @@
         <v>2782</v>
       </c>
       <c r="G16" t="s">
+        <v>43</v>
+      </c>
+      <c r="H16" t="s">
         <v>44</v>
       </c>
-      <c r="H16" t="s">
-        <v>45</v>
-      </c>
       <c r="I16" t="s">
-        <v>21</v>
-      </c>
-      <c r="J16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N16">
+      <c r="M16" t="s">
+        <v>261</v>
+      </c>
+      <c r="N16" t="s">
+        <v>262</v>
+      </c>
+      <c r="P16">
         <v>19</v>
       </c>
-      <c r="O16" t="s">
-        <v>39</v>
-      </c>
-      <c r="P16">
+      <c r="Q16" t="s">
+        <v>38</v>
+      </c>
+      <c r="R16">
         <v>0</v>
       </c>
-      <c r="Q16">
+      <c r="S16">
         <v>108</v>
       </c>
-      <c r="R16">
+      <c r="T16">
         <v>850</v>
       </c>
-      <c r="S16">
+      <c r="U16">
         <v>852</v>
       </c>
-      <c r="T16" t="s">
+      <c r="V16" t="s">
+        <v>219</v>
+      </c>
+      <c r="W16" t="s">
         <v>220</v>
       </c>
-      <c r="U16" t="s">
-        <v>221</v>
-      </c>
-      <c r="V16" t="s">
+      <c r="X16" t="s">
+        <v>258</v>
+      </c>
+      <c r="Y16" t="s">
         <v>259</v>
       </c>
-      <c r="W16" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2652,7 +2765,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17">
         <v>398</v>
@@ -2664,49 +2777,55 @@
         <v>2494</v>
       </c>
       <c r="G17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" t="s">
         <v>46</v>
       </c>
-      <c r="H17" t="s">
-        <v>47</v>
-      </c>
       <c r="I17" t="s">
-        <v>15</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="N17">
+        <v>14</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="M17" t="s">
+        <v>258</v>
+      </c>
+      <c r="N17" t="s">
+        <v>259</v>
+      </c>
+      <c r="P17">
         <v>20</v>
       </c>
-      <c r="O17" t="s">
-        <v>39</v>
-      </c>
-      <c r="P17">
+      <c r="Q17" t="s">
+        <v>38</v>
+      </c>
+      <c r="R17">
         <v>0</v>
       </c>
-      <c r="Q17">
+      <c r="S17">
         <v>22</v>
       </c>
-      <c r="R17">
+      <c r="T17">
         <v>3604</v>
       </c>
-      <c r="S17">
+      <c r="U17">
         <v>3608</v>
       </c>
-      <c r="T17" t="s">
+      <c r="V17" t="s">
+        <v>56</v>
+      </c>
+      <c r="W17" t="s">
         <v>57</v>
       </c>
-      <c r="U17" t="s">
-        <v>58</v>
-      </c>
-      <c r="V17" t="s">
-        <v>259</v>
-      </c>
-      <c r="W17" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X17" t="s">
+        <v>258</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2714,7 +2833,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18">
         <v>70</v>
@@ -2726,19 +2845,25 @@
         <v>1430</v>
       </c>
       <c r="G18" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" t="s">
         <v>48</v>
       </c>
-      <c r="H18" t="s">
-        <v>49</v>
-      </c>
       <c r="I18" t="s">
-        <v>18</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M18" t="s">
+        <v>258</v>
+      </c>
+      <c r="N18" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2746,7 +2871,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19">
         <v>71</v>
@@ -2758,19 +2883,25 @@
         <v>1500</v>
       </c>
       <c r="G19" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" t="s">
         <v>50</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>51</v>
       </c>
-      <c r="I19" t="s">
-        <v>52</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="K19" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="M19" t="s">
+        <v>258</v>
+      </c>
+      <c r="N19" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2778,7 +2909,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20">
         <v>436</v>
@@ -2790,19 +2921,25 @@
         <v>2214</v>
       </c>
       <c r="G20" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" t="s">
         <v>53</v>
       </c>
-      <c r="H20" t="s">
-        <v>54</v>
-      </c>
       <c r="I20" t="s">
-        <v>15</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="M20" t="s">
+        <v>258</v>
+      </c>
+      <c r="N20" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2810,7 +2947,7 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21">
         <v>231</v>
@@ -2822,19 +2959,25 @@
         <v>1896</v>
       </c>
       <c r="G21" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" t="s">
         <v>55</v>
       </c>
-      <c r="H21" t="s">
-        <v>56</v>
-      </c>
       <c r="I21" t="s">
-        <v>28</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="M21" t="s">
+        <v>258</v>
+      </c>
+      <c r="N21" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2842,7 +2985,7 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22">
         <v>22</v>
@@ -2854,22 +2997,28 @@
         <v>3608</v>
       </c>
       <c r="G22" t="s">
+        <v>56</v>
+      </c>
+      <c r="H22" t="s">
         <v>57</v>
       </c>
-      <c r="H22" t="s">
-        <v>58</v>
-      </c>
       <c r="I22" t="s">
-        <v>15</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>248</v>
+        <v>14</v>
       </c>
       <c r="K22" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="L22" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>258</v>
+      </c>
+      <c r="N22" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2877,7 +3026,7 @@
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D23">
         <v>132</v>
@@ -2889,42 +3038,51 @@
         <v>4194</v>
       </c>
       <c r="G23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" t="s">
         <v>59</v>
       </c>
-      <c r="H23" t="s">
-        <v>60</v>
-      </c>
       <c r="I23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="M23" t="s">
+        <v>258</v>
+      </c>
+      <c r="N23" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2932,7 +3090,7 @@
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D25">
         <v>291</v>
@@ -2944,13 +3102,13 @@
         <v>2980</v>
       </c>
       <c r="G25" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" t="s">
         <v>62</v>
       </c>
-      <c r="H25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2958,7 +3116,7 @@
         <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D26">
         <v>32</v>
@@ -2970,13 +3128,13 @@
         <v>340</v>
       </c>
       <c r="G26" t="s">
+        <v>63</v>
+      </c>
+      <c r="H26" t="s">
         <v>64</v>
       </c>
-      <c r="H26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2984,7 +3142,7 @@
         <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D27">
         <v>85</v>
@@ -2996,13 +3154,13 @@
         <v>966</v>
       </c>
       <c r="G27" t="s">
+        <v>65</v>
+      </c>
+      <c r="H27" t="s">
         <v>66</v>
       </c>
-      <c r="H27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3010,7 +3168,7 @@
         <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D28">
         <v>103</v>
@@ -3022,13 +3180,13 @@
         <v>1144</v>
       </c>
       <c r="G28" t="s">
+        <v>67</v>
+      </c>
+      <c r="H28" t="s">
         <v>68</v>
       </c>
-      <c r="H28" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3036,7 +3194,7 @@
         <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D29">
         <v>123</v>
@@ -3048,13 +3206,13 @@
         <v>1372</v>
       </c>
       <c r="G29" t="s">
+        <v>69</v>
+      </c>
+      <c r="H29" t="s">
         <v>70</v>
       </c>
-      <c r="H29" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3062,7 +3220,7 @@
         <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D30">
         <v>129</v>
@@ -3074,13 +3232,13 @@
         <v>1430</v>
       </c>
       <c r="G30" t="s">
+        <v>47</v>
+      </c>
+      <c r="H30" t="s">
         <v>48</v>
       </c>
-      <c r="H30" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3088,7 +3246,7 @@
         <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D31">
         <v>130</v>
@@ -3100,13 +3258,13 @@
         <v>1450</v>
       </c>
       <c r="G31" t="s">
+        <v>71</v>
+      </c>
+      <c r="H31" t="s">
         <v>72</v>
       </c>
-      <c r="H31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3114,7 +3272,7 @@
         <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D32">
         <v>131</v>
@@ -3126,10 +3284,10 @@
         <v>1460</v>
       </c>
       <c r="G32" t="s">
+        <v>73</v>
+      </c>
+      <c r="H32" t="s">
         <v>74</v>
-      </c>
-      <c r="H32" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3140,7 +3298,7 @@
         <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D33">
         <v>132</v>
@@ -3152,10 +3310,10 @@
         <v>1476</v>
       </c>
       <c r="G33" t="s">
+        <v>75</v>
+      </c>
+      <c r="H33" t="s">
         <v>76</v>
-      </c>
-      <c r="H33" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3166,7 +3324,7 @@
         <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D34">
         <v>138</v>
@@ -3178,10 +3336,10 @@
         <v>1542</v>
       </c>
       <c r="G34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3192,7 +3350,7 @@
         <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D35">
         <v>139</v>
@@ -3204,10 +3362,10 @@
         <v>1554</v>
       </c>
       <c r="G35" t="s">
+        <v>78</v>
+      </c>
+      <c r="H35" t="s">
         <v>79</v>
-      </c>
-      <c r="H35" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3218,7 +3376,7 @@
         <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D36">
         <v>140</v>
@@ -3230,10 +3388,10 @@
         <v>1584</v>
       </c>
       <c r="G36" t="s">
+        <v>80</v>
+      </c>
+      <c r="H36" t="s">
         <v>81</v>
-      </c>
-      <c r="H36" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3244,7 +3402,7 @@
         <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D37">
         <v>141</v>
@@ -3256,10 +3414,10 @@
         <v>1592</v>
       </c>
       <c r="G37" t="s">
+        <v>82</v>
+      </c>
+      <c r="H37" t="s">
         <v>83</v>
-      </c>
-      <c r="H37" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3270,7 +3428,7 @@
         <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D38">
         <v>142</v>
@@ -3282,10 +3440,10 @@
         <v>1622</v>
       </c>
       <c r="G38" t="s">
+        <v>84</v>
+      </c>
+      <c r="H38" t="s">
         <v>85</v>
-      </c>
-      <c r="H38" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3296,7 +3454,7 @@
         <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D39">
         <v>143</v>
@@ -3308,10 +3466,10 @@
         <v>1632</v>
       </c>
       <c r="G39" t="s">
+        <v>86</v>
+      </c>
+      <c r="H39" t="s">
         <v>87</v>
-      </c>
-      <c r="H39" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -3322,7 +3480,7 @@
         <v>17</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D40">
         <v>87</v>
@@ -3334,10 +3492,10 @@
         <v>1228</v>
       </c>
       <c r="G40" t="s">
+        <v>88</v>
+      </c>
+      <c r="H40" t="s">
         <v>89</v>
-      </c>
-      <c r="H40" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -3348,7 +3506,7 @@
         <v>17</v>
       </c>
       <c r="C41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D41">
         <v>107</v>
@@ -3360,10 +3518,10 @@
         <v>1340</v>
       </c>
       <c r="G41" t="s">
+        <v>90</v>
+      </c>
+      <c r="H41" t="s">
         <v>91</v>
-      </c>
-      <c r="H41" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3374,7 +3532,7 @@
         <v>17</v>
       </c>
       <c r="C42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D42">
         <v>121</v>
@@ -3386,10 +3544,10 @@
         <v>1464</v>
       </c>
       <c r="G42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -3400,7 +3558,7 @@
         <v>17</v>
       </c>
       <c r="C43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D43">
         <v>125</v>
@@ -3412,10 +3570,10 @@
         <v>1528</v>
       </c>
       <c r="G43" t="s">
+        <v>93</v>
+      </c>
+      <c r="H43" t="s">
         <v>94</v>
-      </c>
-      <c r="H43" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -3426,7 +3584,7 @@
         <v>17</v>
       </c>
       <c r="C44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D44">
         <v>126</v>
@@ -3438,10 +3596,10 @@
         <v>1536</v>
       </c>
       <c r="G44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3452,7 +3610,7 @@
         <v>17</v>
       </c>
       <c r="C45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D45">
         <v>127</v>
@@ -3464,10 +3622,10 @@
         <v>1588</v>
       </c>
       <c r="G45" t="s">
+        <v>96</v>
+      </c>
+      <c r="H45" t="s">
         <v>97</v>
-      </c>
-      <c r="H45" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3478,7 +3636,7 @@
         <v>17</v>
       </c>
       <c r="C46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D46">
         <v>143</v>
@@ -3490,10 +3648,10 @@
         <v>1836</v>
       </c>
       <c r="G46" t="s">
+        <v>98</v>
+      </c>
+      <c r="H46" t="s">
         <v>99</v>
-      </c>
-      <c r="H46" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3504,7 +3662,7 @@
         <v>17</v>
       </c>
       <c r="C47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D47">
         <v>179</v>
@@ -3516,10 +3674,10 @@
         <v>2278</v>
       </c>
       <c r="G47" t="s">
+        <v>100</v>
+      </c>
+      <c r="H47" t="s">
         <v>101</v>
-      </c>
-      <c r="H47" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3530,7 +3688,7 @@
         <v>17</v>
       </c>
       <c r="C48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D48">
         <v>481</v>
@@ -3542,10 +3700,10 @@
         <v>4102</v>
       </c>
       <c r="G48" t="s">
+        <v>102</v>
+      </c>
+      <c r="H48" t="s">
         <v>103</v>
-      </c>
-      <c r="H48" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -3556,7 +3714,7 @@
         <v>17</v>
       </c>
       <c r="C49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D49">
         <v>485</v>
@@ -3568,10 +3726,10 @@
         <v>4138</v>
       </c>
       <c r="G49" t="s">
+        <v>104</v>
+      </c>
+      <c r="H49" t="s">
         <v>105</v>
-      </c>
-      <c r="H49" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -3582,7 +3740,7 @@
         <v>17</v>
       </c>
       <c r="C50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D50">
         <v>486</v>
@@ -3594,10 +3752,10 @@
         <v>4150</v>
       </c>
       <c r="G50" t="s">
+        <v>106</v>
+      </c>
+      <c r="H50" t="s">
         <v>107</v>
-      </c>
-      <c r="H50" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -3608,7 +3766,7 @@
         <v>17</v>
       </c>
       <c r="C51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D51">
         <v>571</v>
@@ -3620,10 +3778,10 @@
         <v>4958</v>
       </c>
       <c r="G51" t="s">
+        <v>108</v>
+      </c>
+      <c r="H51" t="s">
         <v>109</v>
-      </c>
-      <c r="H51" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -3634,7 +3792,7 @@
         <v>18</v>
       </c>
       <c r="C52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D52">
         <v>490</v>
@@ -3646,10 +3804,10 @@
         <v>2252</v>
       </c>
       <c r="G52" t="s">
+        <v>110</v>
+      </c>
+      <c r="H52" t="s">
         <v>111</v>
-      </c>
-      <c r="H52" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -3660,7 +3818,7 @@
         <v>18</v>
       </c>
       <c r="C53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D53">
         <v>495</v>
@@ -3672,10 +3830,10 @@
         <v>2300</v>
       </c>
       <c r="G53" t="s">
+        <v>112</v>
+      </c>
+      <c r="H53" t="s">
         <v>113</v>
-      </c>
-      <c r="H53" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -3686,7 +3844,7 @@
         <v>18</v>
       </c>
       <c r="C54" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D54">
         <v>506</v>
@@ -3698,10 +3856,10 @@
         <v>2312</v>
       </c>
       <c r="G54" t="s">
+        <v>114</v>
+      </c>
+      <c r="H54" t="s">
         <v>115</v>
-      </c>
-      <c r="H54" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -3712,7 +3870,7 @@
         <v>19</v>
       </c>
       <c r="C55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D55">
         <v>199</v>
@@ -3724,10 +3882,10 @@
         <v>1550</v>
       </c>
       <c r="G55" t="s">
+        <v>116</v>
+      </c>
+      <c r="H55" t="s">
         <v>117</v>
-      </c>
-      <c r="H55" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -3738,7 +3896,7 @@
         <v>19</v>
       </c>
       <c r="C56" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D56">
         <v>203</v>
@@ -3750,10 +3908,10 @@
         <v>1556</v>
       </c>
       <c r="G56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H56" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -3764,7 +3922,7 @@
         <v>19</v>
       </c>
       <c r="C57" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D57">
         <v>277</v>
@@ -3776,10 +3934,10 @@
         <v>2002</v>
       </c>
       <c r="G57" t="s">
+        <v>119</v>
+      </c>
+      <c r="H57" t="s">
         <v>120</v>
-      </c>
-      <c r="H57" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -3790,7 +3948,7 @@
         <v>19</v>
       </c>
       <c r="C58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D58">
         <v>280</v>
@@ -3802,10 +3960,10 @@
         <v>2036</v>
       </c>
       <c r="G58" t="s">
+        <v>121</v>
+      </c>
+      <c r="H58" t="s">
         <v>122</v>
-      </c>
-      <c r="H58" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -3816,7 +3974,7 @@
         <v>19</v>
       </c>
       <c r="C59" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D59">
         <v>353</v>
@@ -3828,10 +3986,10 @@
         <v>2468</v>
       </c>
       <c r="G59" t="s">
+        <v>123</v>
+      </c>
+      <c r="H59" t="s">
         <v>124</v>
-      </c>
-      <c r="H59" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -3842,7 +4000,7 @@
         <v>20</v>
       </c>
       <c r="C60" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D60">
         <v>145</v>
@@ -3854,10 +4012,10 @@
         <v>978</v>
       </c>
       <c r="G60" t="s">
+        <v>125</v>
+      </c>
+      <c r="H60" t="s">
         <v>126</v>
-      </c>
-      <c r="H60" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -3868,7 +4026,7 @@
         <v>20</v>
       </c>
       <c r="C61" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D61">
         <v>149</v>
@@ -3880,10 +4038,10 @@
         <v>1014</v>
       </c>
       <c r="G61" t="s">
+        <v>127</v>
+      </c>
+      <c r="H61" t="s">
         <v>128</v>
-      </c>
-      <c r="H61" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -3894,7 +4052,7 @@
         <v>20</v>
       </c>
       <c r="C62" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D62">
         <v>153</v>
@@ -3906,10 +4064,10 @@
         <v>1044</v>
       </c>
       <c r="G62" t="s">
+        <v>129</v>
+      </c>
+      <c r="H62" t="s">
         <v>130</v>
-      </c>
-      <c r="H62" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -3920,7 +4078,7 @@
         <v>20</v>
       </c>
       <c r="C63" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D63">
         <v>159</v>
@@ -3932,10 +4090,10 @@
         <v>1068</v>
       </c>
       <c r="G63" t="s">
+        <v>131</v>
+      </c>
+      <c r="H63" t="s">
         <v>132</v>
-      </c>
-      <c r="H63" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -3946,7 +4104,7 @@
         <v>20</v>
       </c>
       <c r="C64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D64">
         <v>160</v>
@@ -3958,10 +4116,10 @@
         <v>1078</v>
       </c>
       <c r="G64" t="s">
+        <v>133</v>
+      </c>
+      <c r="H64" t="s">
         <v>134</v>
-      </c>
-      <c r="H64" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -3972,7 +4130,7 @@
         <v>20</v>
       </c>
       <c r="C65" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D65">
         <v>161</v>
@@ -3984,10 +4142,10 @@
         <v>1086</v>
       </c>
       <c r="G65" t="s">
+        <v>135</v>
+      </c>
+      <c r="H65" t="s">
         <v>136</v>
-      </c>
-      <c r="H65" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -3998,7 +4156,7 @@
         <v>20</v>
       </c>
       <c r="C66" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D66">
         <v>162</v>
@@ -4010,10 +4168,10 @@
         <v>1104</v>
       </c>
       <c r="G66" t="s">
+        <v>137</v>
+      </c>
+      <c r="H66" t="s">
         <v>138</v>
-      </c>
-      <c r="H66" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -4024,7 +4182,7 @@
         <v>20</v>
       </c>
       <c r="C67" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D67">
         <v>163</v>
@@ -4036,10 +4194,10 @@
         <v>1118</v>
       </c>
       <c r="G67" t="s">
+        <v>139</v>
+      </c>
+      <c r="H67" t="s">
         <v>140</v>
-      </c>
-      <c r="H67" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -4050,7 +4208,7 @@
         <v>20</v>
       </c>
       <c r="C68" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D68">
         <v>164</v>
@@ -4062,10 +4220,10 @@
         <v>1142</v>
       </c>
       <c r="G68" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H68" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -4076,7 +4234,7 @@
         <v>20</v>
       </c>
       <c r="C69" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D69">
         <v>165</v>
@@ -4088,10 +4246,10 @@
         <v>1152</v>
       </c>
       <c r="G69" t="s">
+        <v>141</v>
+      </c>
+      <c r="H69" t="s">
         <v>142</v>
-      </c>
-      <c r="H69" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -4102,7 +4260,7 @@
         <v>20</v>
       </c>
       <c r="C70" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D70">
         <v>167</v>
@@ -4114,10 +4272,10 @@
         <v>1166</v>
       </c>
       <c r="G70" t="s">
+        <v>143</v>
+      </c>
+      <c r="H70" t="s">
         <v>144</v>
-      </c>
-      <c r="H70" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -4128,7 +4286,7 @@
         <v>20</v>
       </c>
       <c r="C71" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D71">
         <v>168</v>
@@ -4140,10 +4298,10 @@
         <v>1184</v>
       </c>
       <c r="G71" t="s">
+        <v>145</v>
+      </c>
+      <c r="H71" t="s">
         <v>146</v>
-      </c>
-      <c r="H71" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -4154,7 +4312,7 @@
         <v>20</v>
       </c>
       <c r="C72" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D72">
         <v>191</v>
@@ -4166,10 +4324,10 @@
         <v>1546</v>
       </c>
       <c r="G72" t="s">
+        <v>147</v>
+      </c>
+      <c r="H72" t="s">
         <v>148</v>
-      </c>
-      <c r="H72" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -4180,7 +4338,7 @@
         <v>20</v>
       </c>
       <c r="C73" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D73">
         <v>209</v>
@@ -4192,10 +4350,10 @@
         <v>1630</v>
       </c>
       <c r="G73" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H73" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -4206,7 +4364,7 @@
         <v>20</v>
       </c>
       <c r="C74" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D74">
         <v>292</v>
@@ -4218,10 +4376,10 @@
         <v>2092</v>
       </c>
       <c r="G74" t="s">
+        <v>150</v>
+      </c>
+      <c r="H74" t="s">
         <v>151</v>
-      </c>
-      <c r="H74" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -4232,7 +4390,7 @@
         <v>20</v>
       </c>
       <c r="C75" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D75">
         <v>387</v>
@@ -4244,10 +4402,10 @@
         <v>2608</v>
       </c>
       <c r="G75" t="s">
+        <v>152</v>
+      </c>
+      <c r="H75" t="s">
         <v>153</v>
-      </c>
-      <c r="H75" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -4258,7 +4416,7 @@
         <v>20</v>
       </c>
       <c r="C76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D76">
         <v>404</v>
@@ -4270,10 +4428,10 @@
         <v>2686</v>
       </c>
       <c r="G76" t="s">
+        <v>154</v>
+      </c>
+      <c r="H76" t="s">
         <v>155</v>
-      </c>
-      <c r="H76" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -4284,7 +4442,7 @@
         <v>20</v>
       </c>
       <c r="C77" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D77">
         <v>415</v>
@@ -4296,10 +4454,10 @@
         <v>2744</v>
       </c>
       <c r="G77" t="s">
+        <v>156</v>
+      </c>
+      <c r="H77" t="s">
         <v>157</v>
-      </c>
-      <c r="H77" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -4310,7 +4468,7 @@
         <v>20</v>
       </c>
       <c r="C78" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D78">
         <v>419</v>
@@ -4322,10 +4480,10 @@
         <v>2752</v>
       </c>
       <c r="G78" t="s">
+        <v>158</v>
+      </c>
+      <c r="H78" t="s">
         <v>159</v>
-      </c>
-      <c r="H78" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -4336,7 +4494,7 @@
         <v>20</v>
       </c>
       <c r="C79" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D79">
         <v>504</v>
@@ -4348,10 +4506,10 @@
         <v>3402</v>
       </c>
       <c r="G79" t="s">
+        <v>160</v>
+      </c>
+      <c r="H79" t="s">
         <v>161</v>
-      </c>
-      <c r="H79" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -4362,7 +4520,7 @@
         <v>2</v>
       </c>
       <c r="C80" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D80">
         <v>133</v>
@@ -4374,10 +4532,10 @@
         <v>2174</v>
       </c>
       <c r="G80" t="s">
+        <v>162</v>
+      </c>
+      <c r="H80" t="s">
         <v>163</v>
-      </c>
-      <c r="H80" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -4388,7 +4546,7 @@
         <v>2</v>
       </c>
       <c r="C81" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D81">
         <v>159</v>
@@ -4400,10 +4558,10 @@
         <v>2386</v>
       </c>
       <c r="G81" t="s">
+        <v>164</v>
+      </c>
+      <c r="H81" t="s">
         <v>165</v>
-      </c>
-      <c r="H81" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -4414,7 +4572,7 @@
         <v>2</v>
       </c>
       <c r="C82" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D82">
         <v>163</v>
@@ -4426,10 +4584,10 @@
         <v>2406</v>
       </c>
       <c r="G82" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H82" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -4440,7 +4598,7 @@
         <v>2</v>
       </c>
       <c r="C83" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D83">
         <v>239</v>
@@ -4452,10 +4610,10 @@
         <v>3256</v>
       </c>
       <c r="G83" t="s">
+        <v>167</v>
+      </c>
+      <c r="H83" t="s">
         <v>168</v>
-      </c>
-      <c r="H83" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -4466,7 +4624,7 @@
         <v>2</v>
       </c>
       <c r="C84" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D84">
         <v>404</v>
@@ -4478,10 +4636,10 @@
         <v>4772</v>
       </c>
       <c r="G84" t="s">
+        <v>169</v>
+      </c>
+      <c r="H84" t="s">
         <v>170</v>
-      </c>
-      <c r="H84" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -4492,7 +4650,7 @@
         <v>2</v>
       </c>
       <c r="C85" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D85">
         <v>409</v>
@@ -4504,10 +4662,10 @@
         <v>4794</v>
       </c>
       <c r="G85" t="s">
+        <v>171</v>
+      </c>
+      <c r="H85" t="s">
         <v>172</v>
-      </c>
-      <c r="H85" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -4518,7 +4676,7 @@
         <v>12</v>
       </c>
       <c r="C86" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D86">
         <v>49</v>
@@ -4530,10 +4688,10 @@
         <v>506</v>
       </c>
       <c r="G86" t="s">
+        <v>173</v>
+      </c>
+      <c r="H86" t="s">
         <v>174</v>
-      </c>
-      <c r="H86" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -4544,7 +4702,7 @@
         <v>12</v>
       </c>
       <c r="C87" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D87">
         <v>50</v>
@@ -4556,10 +4714,10 @@
         <v>512</v>
       </c>
       <c r="G87" t="s">
+        <v>175</v>
+      </c>
+      <c r="H87" t="s">
         <v>176</v>
-      </c>
-      <c r="H87" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -4570,7 +4728,7 @@
         <v>12</v>
       </c>
       <c r="C88" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D88">
         <v>160</v>
@@ -4582,10 +4740,10 @@
         <v>1962</v>
       </c>
       <c r="G88" t="s">
+        <v>177</v>
+      </c>
+      <c r="H88" t="s">
         <v>178</v>
-      </c>
-      <c r="H88" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -4596,7 +4754,7 @@
         <v>12</v>
       </c>
       <c r="C89" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D89">
         <v>203</v>
@@ -4608,10 +4766,10 @@
         <v>2292</v>
       </c>
       <c r="G89" t="s">
+        <v>179</v>
+      </c>
+      <c r="H89" t="s">
         <v>180</v>
-      </c>
-      <c r="H89" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -4622,7 +4780,7 @@
         <v>12</v>
       </c>
       <c r="C90" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D90">
         <v>209</v>
@@ -4634,10 +4792,10 @@
         <v>2334</v>
       </c>
       <c r="G90" t="s">
+        <v>181</v>
+      </c>
+      <c r="H90" t="s">
         <v>182</v>
-      </c>
-      <c r="H90" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -4648,7 +4806,7 @@
         <v>12</v>
       </c>
       <c r="C91" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D91">
         <v>526</v>
@@ -4660,10 +4818,10 @@
         <v>7146</v>
       </c>
       <c r="G91" t="s">
+        <v>183</v>
+      </c>
+      <c r="H91" t="s">
         <v>184</v>
-      </c>
-      <c r="H91" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -4674,7 +4832,7 @@
         <v>17</v>
       </c>
       <c r="C92" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D92">
         <v>55</v>
@@ -4686,10 +4844,10 @@
         <v>1044</v>
       </c>
       <c r="G92" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H92" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -4700,7 +4858,7 @@
         <v>17</v>
       </c>
       <c r="C93" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D93">
         <v>59</v>
@@ -4712,10 +4870,10 @@
         <v>1106</v>
       </c>
       <c r="G93" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H93" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -4726,7 +4884,7 @@
         <v>17</v>
       </c>
       <c r="C94" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D94">
         <v>61</v>
@@ -4738,10 +4896,10 @@
         <v>1188</v>
       </c>
       <c r="G94" t="s">
+        <v>187</v>
+      </c>
+      <c r="H94" t="s">
         <v>188</v>
-      </c>
-      <c r="H94" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -4752,7 +4910,7 @@
         <v>17</v>
       </c>
       <c r="C95" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D95">
         <v>64</v>
@@ -4764,10 +4922,10 @@
         <v>1222</v>
       </c>
       <c r="G95" t="s">
+        <v>189</v>
+      </c>
+      <c r="H95" t="s">
         <v>190</v>
-      </c>
-      <c r="H95" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -4778,7 +4936,7 @@
         <v>17</v>
       </c>
       <c r="C96" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D96">
         <v>65</v>
@@ -4790,10 +4948,10 @@
         <v>1262</v>
       </c>
       <c r="G96" t="s">
+        <v>191</v>
+      </c>
+      <c r="H96" t="s">
         <v>192</v>
-      </c>
-      <c r="H96" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -4804,7 +4962,7 @@
         <v>17</v>
       </c>
       <c r="C97" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D97">
         <v>66</v>
@@ -4816,10 +4974,10 @@
         <v>1274</v>
       </c>
       <c r="G97" t="s">
+        <v>193</v>
+      </c>
+      <c r="H97" t="s">
         <v>194</v>
-      </c>
-      <c r="H97" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -4830,7 +4988,7 @@
         <v>17</v>
       </c>
       <c r="C98" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D98">
         <v>67</v>
@@ -4842,10 +5000,10 @@
         <v>1302</v>
       </c>
       <c r="G98" t="s">
+        <v>195</v>
+      </c>
+      <c r="H98" t="s">
         <v>196</v>
-      </c>
-      <c r="H98" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -4856,7 +5014,7 @@
         <v>17</v>
       </c>
       <c r="C99" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D99">
         <v>68</v>
@@ -4868,10 +5026,10 @@
         <v>1354</v>
       </c>
       <c r="G99" t="s">
+        <v>197</v>
+      </c>
+      <c r="H99" t="s">
         <v>198</v>
-      </c>
-      <c r="H99" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -4882,7 +5040,7 @@
         <v>17</v>
       </c>
       <c r="C100" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D100">
         <v>69</v>
@@ -4894,10 +5052,10 @@
         <v>1388</v>
       </c>
       <c r="G100" t="s">
+        <v>199</v>
+      </c>
+      <c r="H100" t="s">
         <v>200</v>
-      </c>
-      <c r="H100" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -4908,7 +5066,7 @@
         <v>17</v>
       </c>
       <c r="C101" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D101">
         <v>474</v>
@@ -4920,10 +5078,10 @@
         <v>4974</v>
       </c>
       <c r="G101" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H101" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -4934,7 +5092,7 @@
         <v>17</v>
       </c>
       <c r="C102" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D102">
         <v>504</v>
@@ -4946,10 +5104,10 @@
         <v>5138</v>
       </c>
       <c r="G102" t="s">
+        <v>202</v>
+      </c>
+      <c r="H102" t="s">
         <v>203</v>
-      </c>
-      <c r="H102" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -4960,7 +5118,7 @@
         <v>17</v>
       </c>
       <c r="C103" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D103">
         <v>509</v>
@@ -4972,10 +5130,10 @@
         <v>5152</v>
       </c>
       <c r="G103" t="s">
+        <v>204</v>
+      </c>
+      <c r="H103" t="s">
         <v>205</v>
-      </c>
-      <c r="H103" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -4986,7 +5144,7 @@
         <v>17</v>
       </c>
       <c r="C104" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D104">
         <v>510</v>
@@ -4998,10 +5156,10 @@
         <v>5168</v>
       </c>
       <c r="G104" t="s">
+        <v>206</v>
+      </c>
+      <c r="H104" t="s">
         <v>207</v>
-      </c>
-      <c r="H104" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -5012,7 +5170,7 @@
         <v>18</v>
       </c>
       <c r="C105" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D105">
         <v>228</v>
@@ -5024,10 +5182,10 @@
         <v>1356</v>
       </c>
       <c r="G105" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H105" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -5038,7 +5196,7 @@
         <v>18</v>
       </c>
       <c r="C106" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D106">
         <v>239</v>
@@ -5050,10 +5208,10 @@
         <v>1370</v>
       </c>
       <c r="G106" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H106" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -5064,7 +5222,7 @@
         <v>18</v>
       </c>
       <c r="C107" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D107">
         <v>245</v>
@@ -5076,10 +5234,10 @@
         <v>1444</v>
       </c>
       <c r="G107" t="s">
+        <v>210</v>
+      </c>
+      <c r="H107" t="s">
         <v>211</v>
-      </c>
-      <c r="H107" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -5090,7 +5248,7 @@
         <v>18</v>
       </c>
       <c r="C108" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D108">
         <v>256</v>
@@ -5102,10 +5260,10 @@
         <v>1548</v>
       </c>
       <c r="G108" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H108" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -5116,7 +5274,7 @@
         <v>18</v>
       </c>
       <c r="C109" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D109">
         <v>268</v>
@@ -5128,10 +5286,10 @@
         <v>1612</v>
       </c>
       <c r="G109" t="s">
+        <v>212</v>
+      </c>
+      <c r="H109" t="s">
         <v>213</v>
-      </c>
-      <c r="H109" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -5142,7 +5300,7 @@
         <v>18</v>
       </c>
       <c r="C110" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D110">
         <v>341</v>
@@ -5154,10 +5312,10 @@
         <v>1818</v>
       </c>
       <c r="G110" t="s">
+        <v>214</v>
+      </c>
+      <c r="H110" t="s">
         <v>215</v>
-      </c>
-      <c r="H110" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -5168,7 +5326,7 @@
         <v>18</v>
       </c>
       <c r="C111" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D111">
         <v>379</v>
@@ -5180,10 +5338,10 @@
         <v>1924</v>
       </c>
       <c r="G111" t="s">
+        <v>216</v>
+      </c>
+      <c r="H111" t="s">
         <v>217</v>
-      </c>
-      <c r="H111" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -5194,7 +5352,7 @@
         <v>18</v>
       </c>
       <c r="C112" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D112">
         <v>448</v>
@@ -5206,10 +5364,10 @@
         <v>2280</v>
       </c>
       <c r="G112" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H112" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -5220,7 +5378,7 @@
         <v>19</v>
       </c>
       <c r="C113" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D113">
         <v>108</v>
@@ -5232,10 +5390,10 @@
         <v>852</v>
       </c>
       <c r="G113" t="s">
+        <v>219</v>
+      </c>
+      <c r="H113" t="s">
         <v>220</v>
-      </c>
-      <c r="H113" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -5246,7 +5404,7 @@
         <v>19</v>
       </c>
       <c r="C114" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D114">
         <v>112</v>
@@ -5258,10 +5416,10 @@
         <v>936</v>
       </c>
       <c r="G114" t="s">
+        <v>221</v>
+      </c>
+      <c r="H114" t="s">
         <v>222</v>
-      </c>
-      <c r="H114" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -5272,7 +5430,7 @@
         <v>19</v>
       </c>
       <c r="C115" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D115">
         <v>115</v>
@@ -5284,10 +5442,10 @@
         <v>1008</v>
       </c>
       <c r="G115" t="s">
+        <v>223</v>
+      </c>
+      <c r="H115" t="s">
         <v>224</v>
-      </c>
-      <c r="H115" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -5298,7 +5456,7 @@
         <v>19</v>
       </c>
       <c r="C116" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D116">
         <v>199</v>
@@ -5310,10 +5468,10 @@
         <v>1628</v>
       </c>
       <c r="G116" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H116" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -5324,7 +5482,7 @@
         <v>20</v>
       </c>
       <c r="C117" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D117">
         <v>33</v>
@@ -5336,10 +5494,10 @@
         <v>3656</v>
       </c>
       <c r="G117" t="s">
+        <v>225</v>
+      </c>
+      <c r="H117" t="s">
         <v>226</v>
-      </c>
-      <c r="H117" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -5350,7 +5508,7 @@
         <v>20</v>
       </c>
       <c r="C118" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D118">
         <v>35</v>
@@ -5362,10 +5520,10 @@
         <v>3676</v>
       </c>
       <c r="G118" t="s">
+        <v>227</v>
+      </c>
+      <c r="H118" t="s">
         <v>228</v>
-      </c>
-      <c r="H118" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -5376,7 +5534,7 @@
         <v>20</v>
       </c>
       <c r="C119" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D119">
         <v>43</v>
@@ -5388,10 +5546,10 @@
         <v>3704</v>
       </c>
       <c r="G119" t="s">
+        <v>229</v>
+      </c>
+      <c r="H119" t="s">
         <v>230</v>
-      </c>
-      <c r="H119" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -5402,7 +5560,7 @@
         <v>20</v>
       </c>
       <c r="C120" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D120">
         <v>64</v>
@@ -5414,10 +5572,10 @@
         <v>3814</v>
       </c>
       <c r="G120" t="s">
+        <v>231</v>
+      </c>
+      <c r="H120" t="s">
         <v>232</v>
-      </c>
-      <c r="H120" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -5428,7 +5586,7 @@
         <v>20</v>
       </c>
       <c r="C121" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D121">
         <v>67</v>
@@ -5440,10 +5598,10 @@
         <v>3836</v>
       </c>
       <c r="G121" t="s">
+        <v>233</v>
+      </c>
+      <c r="H121" t="s">
         <v>234</v>
-      </c>
-      <c r="H121" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -5454,7 +5612,7 @@
         <v>20</v>
       </c>
       <c r="C122" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D122">
         <v>88</v>
@@ -5466,10 +5624,10 @@
         <v>3970</v>
       </c>
       <c r="G122" t="s">
+        <v>235</v>
+      </c>
+      <c r="H122" t="s">
         <v>236</v>
-      </c>
-      <c r="H122" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -5480,7 +5638,7 @@
         <v>20</v>
       </c>
       <c r="C123" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D123">
         <v>124</v>
@@ -5492,10 +5650,10 @@
         <v>4140</v>
       </c>
       <c r="G123" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H123" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -5506,7 +5664,7 @@
         <v>20</v>
       </c>
       <c r="C124" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D124">
         <v>129</v>
@@ -5518,10 +5676,10 @@
         <v>4158</v>
       </c>
       <c r="G124" t="s">
+        <v>238</v>
+      </c>
+      <c r="H124" t="s">
         <v>239</v>
-      </c>
-      <c r="H124" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -5532,7 +5690,7 @@
         <v>20</v>
       </c>
       <c r="C125" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D125">
         <v>130</v>
@@ -5544,10 +5702,10 @@
         <v>4172</v>
       </c>
       <c r="G125" t="s">
+        <v>240</v>
+      </c>
+      <c r="H125" t="s">
         <v>241</v>
-      </c>
-      <c r="H125" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -5558,7 +5716,7 @@
         <v>20</v>
       </c>
       <c r="C126" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D126">
         <v>154</v>
@@ -5570,10 +5728,10 @@
         <v>4442</v>
       </c>
       <c r="G126" t="s">
+        <v>242</v>
+      </c>
+      <c r="H126" t="s">
         <v>243</v>
-      </c>
-      <c r="H126" t="s">
-        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>